<commit_message>
Will Start: Working with image cell click
</commit_message>
<xml_diff>
--- a/simple_input.xlsx
+++ b/simple_input.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pankaj/Downloads/GitProjects/SimpleNoteTakingProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC677983-446A-944E-A8F5-E00FC108F0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A98413A-3F23-084D-8956-164C02DF88D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24500" windowHeight="15500" xr2:uid="{0359AB34-A994-0148-BC97-AD51A95FD456}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0359AB34-A994-0148-BC97-AD51A95FD456}"/>
   </bookViews>
   <sheets>
     <sheet name="Function in Details" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="254">
   <si>
     <t>Important Code</t>
   </si>
@@ -1078,6 +1078,12 @@
   </si>
   <si>
     <t>Reference2</t>
+  </si>
+  <si>
+    <t>IMGee</t>
+  </si>
+  <si>
+    <t>[ImageHello](https://res.cloudinary.com/practicaldev/image/fetch/s--Y1v6aJBu--/c_imagga_scale,f_auto,fl_progressive,h_900,q_auto,w_1600/https://thepracticaldev.s3.amazonaws.com/i/ek7ji4zrimozpp2yzk0a.png)</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D33AE3-D714-3B43-9690-2415AEEE2B49}">
   <dimension ref="B3:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1572,8 +1578,8 @@
       <c r="D7" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>250</v>
+      <c r="F7" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>249</v>
@@ -1591,7 +1597,7 @@
         <v>208</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>251</v>
@@ -1710,8 +1716,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{55107A48-0740-8B44-804F-45D58BCD4BD5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>